<commit_message>
Rose - hotel guest - update working, archiving not but it does build
</commit_message>
<xml_diff>
--- a/OfficialInternalBacklog.xlsx
+++ b/OfficialInternalBacklog.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pat B\Google Drive\Capstone Project (Internal)\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" tabRatio="268"/>
   </bookViews>
@@ -30,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="203">
   <si>
     <t>Sprint</t>
   </si>
@@ -637,6 +632,9 @@
   <si>
     <t>Tony/Ryan</t>
   </si>
+  <si>
+    <t>parameters not wanting to be placed in the stored procedure</t>
+  </si>
 </sst>
 </file>
 
@@ -894,10 +892,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -940,6 +934,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1212,7 +1210,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1223,8 +1221,8 @@
   <dimension ref="A1:I1033"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E57" sqref="E57"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1270,946 +1268,960 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="55" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A2" s="51">
+    <row r="2" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A2" s="49">
         <v>2</v>
       </c>
-      <c r="B2" s="52">
+      <c r="B2" s="50">
         <v>1</v>
       </c>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="53" t="s">
+      <c r="D2" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="54" t="s">
+      <c r="E2" s="52" t="s">
         <v>164</v>
       </c>
-      <c r="F2" s="54"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52" t="s">
+      <c r="F2" s="52"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="53" t="s">
+      <c r="I2" s="51" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="55" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A3" s="63"/>
-      <c r="B3" s="64"/>
-      <c r="C3" s="58" t="s">
+    <row r="3" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A3" s="61"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="58" t="s">
+      <c r="D3" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="59" t="s">
+      <c r="E3" s="57" t="s">
         <v>195</v>
       </c>
-      <c r="F3" s="59"/>
-      <c r="G3" s="64" t="s">
+      <c r="F3" s="57"/>
+      <c r="G3" s="62" t="s">
         <v>194</v>
       </c>
-      <c r="H3" s="64"/>
-      <c r="I3" s="59"/>
-    </row>
-    <row r="4" spans="1:9" s="55" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A4" s="63"/>
-      <c r="B4" s="64"/>
-      <c r="C4" s="58" t="s">
+      <c r="H3" s="62"/>
+      <c r="I3" s="57"/>
+    </row>
+    <row r="4" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A4" s="61"/>
+      <c r="B4" s="62"/>
+      <c r="C4" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="58" t="s">
+      <c r="D4" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="59" t="s">
+      <c r="E4" s="57" t="s">
         <v>196</v>
       </c>
-      <c r="F4" s="59"/>
-      <c r="G4" s="64" t="s">
+      <c r="F4" s="57"/>
+      <c r="G4" s="62" t="s">
         <v>194</v>
       </c>
-      <c r="H4" s="64"/>
-      <c r="I4" s="59"/>
-    </row>
-    <row r="5" spans="1:9" s="55" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A5" s="63"/>
-      <c r="B5" s="64"/>
-      <c r="C5" s="58" t="s">
+      <c r="H4" s="62"/>
+      <c r="I4" s="57"/>
+    </row>
+    <row r="5" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A5" s="61"/>
+      <c r="B5" s="62"/>
+      <c r="C5" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="58" t="s">
+      <c r="D5" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="59" t="s">
+      <c r="E5" s="57" t="s">
         <v>197</v>
       </c>
-      <c r="F5" s="59"/>
-      <c r="G5" s="64" t="s">
+      <c r="F5" s="57"/>
+      <c r="G5" s="62" t="s">
         <v>194</v>
       </c>
-      <c r="H5" s="64"/>
-      <c r="I5" s="59"/>
-    </row>
-    <row r="6" spans="1:9" s="55" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="56"/>
-      <c r="B6" s="57"/>
-      <c r="C6" s="58" t="s">
+      <c r="H5" s="62"/>
+      <c r="I5" s="57"/>
+    </row>
+    <row r="6" spans="1:9" s="53" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="54"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="58" t="s">
+      <c r="D6" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="59" t="s">
+      <c r="E6" s="57" t="s">
         <v>198</v>
       </c>
-      <c r="F6" s="60"/>
-      <c r="G6" s="64" t="s">
+      <c r="F6" s="58"/>
+      <c r="G6" s="62" t="s">
         <v>194</v>
       </c>
-      <c r="H6" s="61"/>
-      <c r="I6" s="62"/>
-    </row>
-    <row r="7" spans="1:9" s="55" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A7" s="51">
+      <c r="H6" s="59"/>
+      <c r="I6" s="60"/>
+    </row>
+    <row r="7" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A7" s="49">
         <v>2</v>
       </c>
-      <c r="B7" s="52">
+      <c r="B7" s="50">
         <v>2</v>
       </c>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="53" t="s">
+      <c r="D7" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="E7" s="54" t="s">
+      <c r="E7" s="52" t="s">
         <v>155</v>
       </c>
-      <c r="F7" s="54"/>
-      <c r="G7" s="52"/>
-      <c r="H7" s="52" t="s">
+      <c r="F7" s="52"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="53" t="s">
+      <c r="I7" s="51" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="55" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A8" s="63"/>
-      <c r="B8" s="64"/>
-      <c r="C8" s="58" t="s">
+    <row r="8" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A8" s="61"/>
+      <c r="B8" s="62"/>
+      <c r="C8" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="58" t="s">
+      <c r="D8" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="59" t="s">
+      <c r="E8" s="57" t="s">
         <v>174</v>
       </c>
-      <c r="F8" s="59"/>
-      <c r="G8" s="64" t="s">
+      <c r="F8" s="57"/>
+      <c r="G8" s="62" t="s">
         <v>165</v>
       </c>
-      <c r="H8" s="64"/>
-      <c r="I8" s="59"/>
-    </row>
-    <row r="9" spans="1:9" s="55" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A9" s="63"/>
-      <c r="B9" s="64"/>
-      <c r="C9" s="58" t="s">
+      <c r="H8" s="62"/>
+      <c r="I8" s="57"/>
+    </row>
+    <row r="9" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A9" s="61"/>
+      <c r="B9" s="62"/>
+      <c r="C9" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="58" t="s">
+      <c r="D9" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="59" t="s">
+      <c r="E9" s="57" t="s">
         <v>173</v>
       </c>
-      <c r="F9" s="59"/>
-      <c r="G9" s="64" t="s">
+      <c r="F9" s="57"/>
+      <c r="G9" s="62" t="s">
         <v>165</v>
       </c>
-      <c r="H9" s="64"/>
-      <c r="I9" s="59"/>
-    </row>
-    <row r="10" spans="1:9" s="55" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A10" s="63"/>
-      <c r="B10" s="64"/>
-      <c r="C10" s="58" t="s">
+      <c r="H9" s="62"/>
+      <c r="I9" s="57"/>
+    </row>
+    <row r="10" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A10" s="61"/>
+      <c r="B10" s="62"/>
+      <c r="C10" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="58" t="s">
+      <c r="D10" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="59" t="s">
+      <c r="E10" s="57" t="s">
         <v>182</v>
       </c>
-      <c r="F10" s="59"/>
-      <c r="G10" s="64" t="s">
+      <c r="F10" s="57"/>
+      <c r="G10" s="62" t="s">
         <v>165</v>
       </c>
-      <c r="H10" s="64"/>
-      <c r="I10" s="59"/>
-    </row>
-    <row r="11" spans="1:9" s="55" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A11" s="63"/>
-      <c r="B11" s="64"/>
-      <c r="C11" s="58" t="s">
+      <c r="H10" s="62"/>
+      <c r="I10" s="57"/>
+    </row>
+    <row r="11" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A11" s="61"/>
+      <c r="B11" s="62"/>
+      <c r="C11" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="58" t="s">
+      <c r="D11" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="59" t="s">
+      <c r="E11" s="57" t="s">
         <v>183</v>
       </c>
-      <c r="F11" s="59"/>
-      <c r="G11" s="64" t="s">
+      <c r="F11" s="57"/>
+      <c r="G11" s="62" t="s">
         <v>165</v>
       </c>
-      <c r="H11" s="64"/>
-      <c r="I11" s="59"/>
-    </row>
-    <row r="12" spans="1:9" s="55" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A12" s="63"/>
-      <c r="B12" s="64"/>
-      <c r="C12" s="58" t="s">
+      <c r="H11" s="62"/>
+      <c r="I11" s="57"/>
+    </row>
+    <row r="12" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A12" s="61"/>
+      <c r="B12" s="62"/>
+      <c r="C12" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="58" t="s">
+      <c r="D12" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="59" t="s">
+      <c r="E12" s="57" t="s">
         <v>184</v>
       </c>
-      <c r="F12" s="59"/>
-      <c r="G12" s="64" t="s">
+      <c r="F12" s="57"/>
+      <c r="G12" s="62" t="s">
         <v>165</v>
       </c>
-      <c r="H12" s="64"/>
-      <c r="I12" s="59"/>
-    </row>
-    <row r="13" spans="1:9" s="55" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A13" s="63"/>
-      <c r="B13" s="64"/>
-      <c r="C13" s="58" t="s">
+      <c r="H12" s="62"/>
+      <c r="I12" s="57"/>
+    </row>
+    <row r="13" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A13" s="61"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="58" t="s">
+      <c r="D13" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="59" t="s">
+      <c r="E13" s="57" t="s">
         <v>185</v>
       </c>
-      <c r="F13" s="59"/>
-      <c r="G13" s="64" t="s">
+      <c r="F13" s="57"/>
+      <c r="G13" s="62" t="s">
         <v>165</v>
       </c>
-      <c r="H13" s="64"/>
-      <c r="I13" s="59"/>
-    </row>
-    <row r="14" spans="1:9" s="55" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A14" s="63"/>
-      <c r="B14" s="64"/>
-      <c r="C14" s="58" t="s">
+      <c r="H13" s="62"/>
+      <c r="I13" s="57"/>
+    </row>
+    <row r="14" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A14" s="61"/>
+      <c r="B14" s="62"/>
+      <c r="C14" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="58" t="s">
+      <c r="D14" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="59" t="s">
+      <c r="E14" s="57" t="s">
         <v>166</v>
       </c>
-      <c r="F14" s="59"/>
-      <c r="G14" s="64" t="s">
+      <c r="F14" s="57"/>
+      <c r="G14" s="62" t="s">
         <v>165</v>
       </c>
-      <c r="H14" s="64"/>
-      <c r="I14" s="59"/>
-    </row>
-    <row r="15" spans="1:9" s="55" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A15" s="63"/>
-      <c r="B15" s="64"/>
-      <c r="C15" s="58" t="s">
+      <c r="H14" s="62"/>
+      <c r="I14" s="57"/>
+    </row>
+    <row r="15" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A15" s="61"/>
+      <c r="B15" s="62"/>
+      <c r="C15" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="58" t="s">
+      <c r="D15" s="56" t="s">
         <v>157</v>
       </c>
-      <c r="E15" s="59" t="s">
+      <c r="E15" s="57" t="s">
         <v>153</v>
       </c>
-      <c r="F15" s="59"/>
-      <c r="G15" s="64" t="s">
+      <c r="F15" s="57"/>
+      <c r="G15" s="62" t="s">
         <v>69</v>
       </c>
-      <c r="H15" s="64"/>
-      <c r="I15" s="59" t="s">
+      <c r="H15" s="62"/>
+      <c r="I15" s="57" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="55" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="63"/>
-      <c r="B16" s="64"/>
-      <c r="C16" s="58" t="s">
+    <row r="16" spans="1:9" s="53" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A16" s="61"/>
+      <c r="B16" s="62"/>
+      <c r="C16" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="58" t="s">
+      <c r="D16" s="56" t="s">
         <v>157</v>
       </c>
-      <c r="E16" s="59" t="s">
+      <c r="E16" s="57" t="s">
         <v>167</v>
       </c>
-      <c r="F16" s="59"/>
-      <c r="G16" s="64" t="s">
+      <c r="F16" s="57"/>
+      <c r="G16" s="62" t="s">
         <v>165</v>
       </c>
-      <c r="H16" s="64"/>
-      <c r="I16" s="59"/>
-    </row>
-    <row r="17" spans="1:9" s="55" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="63"/>
-      <c r="B17" s="64"/>
-      <c r="C17" s="58" t="s">
+      <c r="H16" s="62"/>
+      <c r="I16" s="57"/>
+    </row>
+    <row r="17" spans="1:9" s="53" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A17" s="61"/>
+      <c r="B17" s="62"/>
+      <c r="C17" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="58" t="s">
+      <c r="D17" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="59" t="s">
+      <c r="E17" s="57" t="s">
         <v>170</v>
       </c>
-      <c r="F17" s="59"/>
-      <c r="G17" s="64" t="s">
+      <c r="F17" s="57"/>
+      <c r="G17" s="62" t="s">
         <v>165</v>
       </c>
-      <c r="H17" s="64"/>
-      <c r="I17" s="59"/>
-    </row>
-    <row r="18" spans="1:9" s="55" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="63"/>
-      <c r="B18" s="64"/>
-      <c r="C18" s="58" t="s">
+      <c r="H17" s="62"/>
+      <c r="I17" s="57"/>
+    </row>
+    <row r="18" spans="1:9" s="53" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A18" s="61"/>
+      <c r="B18" s="62"/>
+      <c r="C18" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="58" t="s">
+      <c r="D18" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="59" t="s">
+      <c r="E18" s="57" t="s">
         <v>171</v>
       </c>
-      <c r="F18" s="59"/>
-      <c r="G18" s="64" t="s">
+      <c r="F18" s="57"/>
+      <c r="G18" s="62" t="s">
         <v>165</v>
       </c>
-      <c r="H18" s="64"/>
-      <c r="I18" s="59"/>
-    </row>
-    <row r="19" spans="1:9" s="55" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A19" s="51">
+      <c r="H18" s="62"/>
+      <c r="I18" s="57"/>
+    </row>
+    <row r="19" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A19" s="49">
         <v>2</v>
       </c>
-      <c r="B19" s="52">
+      <c r="B19" s="50">
         <v>2</v>
       </c>
-      <c r="C19" s="53" t="s">
+      <c r="C19" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="53" t="s">
+      <c r="D19" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="E19" s="54" t="s">
+      <c r="E19" s="52" t="s">
         <v>156</v>
       </c>
-      <c r="F19" s="54"/>
-      <c r="G19" s="52"/>
-      <c r="H19" s="52" t="s">
+      <c r="F19" s="52"/>
+      <c r="G19" s="50"/>
+      <c r="H19" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="53" t="s">
+      <c r="I19" s="51" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="55" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A20" s="63"/>
-      <c r="B20" s="64"/>
-      <c r="C20" s="58" t="s">
+    <row r="20" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A20" s="61"/>
+      <c r="B20" s="62"/>
+      <c r="C20" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="58" t="s">
+      <c r="D20" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="59" t="s">
+      <c r="E20" s="57" t="s">
         <v>175</v>
       </c>
-      <c r="F20" s="59"/>
-      <c r="G20" s="64" t="s">
+      <c r="F20" s="57"/>
+      <c r="G20" s="62" t="s">
         <v>165</v>
       </c>
-      <c r="H20" s="64"/>
-      <c r="I20" s="59"/>
-    </row>
-    <row r="21" spans="1:9" s="55" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A21" s="63"/>
-      <c r="B21" s="64"/>
-      <c r="C21" s="58" t="s">
+      <c r="H20" s="62"/>
+      <c r="I20" s="57" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A21" s="61"/>
+      <c r="B21" s="62"/>
+      <c r="C21" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="58" t="s">
+      <c r="D21" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="E21" s="59" t="s">
+      <c r="E21" s="57" t="s">
         <v>176</v>
       </c>
-      <c r="F21" s="59"/>
-      <c r="G21" s="64" t="s">
+      <c r="F21" s="57"/>
+      <c r="G21" s="62" t="s">
         <v>165</v>
       </c>
-      <c r="H21" s="64"/>
-      <c r="I21" s="59"/>
-    </row>
-    <row r="22" spans="1:9" s="55" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A22" s="63"/>
-      <c r="B22" s="64"/>
-      <c r="C22" s="58" t="s">
+      <c r="H21" s="62"/>
+      <c r="I21" s="57" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A22" s="61"/>
+      <c r="B22" s="62"/>
+      <c r="C22" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="58" t="s">
+      <c r="D22" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="E22" s="59" t="s">
+      <c r="E22" s="57" t="s">
         <v>180</v>
       </c>
-      <c r="F22" s="59"/>
-      <c r="G22" s="64" t="s">
+      <c r="F22" s="57"/>
+      <c r="G22" s="62" t="s">
         <v>165</v>
       </c>
-      <c r="H22" s="64"/>
-      <c r="I22" s="59"/>
-    </row>
-    <row r="23" spans="1:9" s="55" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A23" s="63"/>
-      <c r="B23" s="64"/>
-      <c r="C23" s="58" t="s">
+      <c r="H22" s="62"/>
+      <c r="I22" s="57" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A23" s="61"/>
+      <c r="B23" s="62"/>
+      <c r="C23" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D23" s="58" t="s">
+      <c r="D23" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="E23" s="59" t="s">
+      <c r="E23" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="F23" s="59"/>
-      <c r="G23" s="64" t="s">
+      <c r="F23" s="57" t="s">
+        <v>202</v>
+      </c>
+      <c r="G23" s="62" t="s">
         <v>165</v>
       </c>
-      <c r="H23" s="64"/>
-      <c r="I23" s="59"/>
-    </row>
-    <row r="24" spans="1:9" s="55" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A24" s="63"/>
-      <c r="B24" s="64"/>
-      <c r="C24" s="58" t="s">
+      <c r="H23" s="62"/>
+      <c r="I23" s="57"/>
+    </row>
+    <row r="24" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A24" s="61"/>
+      <c r="B24" s="62"/>
+      <c r="C24" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D24" s="58" t="s">
+      <c r="D24" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="E24" s="59" t="s">
+      <c r="E24" s="57" t="s">
         <v>178</v>
       </c>
-      <c r="F24" s="59"/>
-      <c r="G24" s="64" t="s">
+      <c r="F24" s="57"/>
+      <c r="G24" s="62" t="s">
         <v>165</v>
       </c>
-      <c r="H24" s="64"/>
-      <c r="I24" s="59"/>
-    </row>
-    <row r="25" spans="1:9" s="55" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A25" s="63"/>
-      <c r="B25" s="64"/>
-      <c r="C25" s="58" t="s">
+      <c r="H24" s="62"/>
+      <c r="I24" s="57" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A25" s="61"/>
+      <c r="B25" s="62"/>
+      <c r="C25" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="58" t="s">
+      <c r="D25" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="E25" s="59" t="s">
+      <c r="E25" s="57" t="s">
         <v>179</v>
       </c>
-      <c r="F25" s="59"/>
-      <c r="G25" s="64" t="s">
+      <c r="F25" s="57"/>
+      <c r="G25" s="62" t="s">
         <v>165</v>
       </c>
-      <c r="H25" s="64"/>
-      <c r="I25" s="59"/>
-    </row>
-    <row r="26" spans="1:9" s="55" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A26" s="63"/>
-      <c r="B26" s="64"/>
-      <c r="C26" s="58" t="s">
+      <c r="H25" s="62"/>
+      <c r="I25" s="57" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A26" s="61"/>
+      <c r="B26" s="62"/>
+      <c r="C26" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D26" s="58" t="s">
+      <c r="D26" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="E26" s="59" t="s">
+      <c r="E26" s="57" t="s">
         <v>163</v>
       </c>
-      <c r="F26" s="59"/>
-      <c r="G26" s="64" t="s">
+      <c r="F26" s="57"/>
+      <c r="G26" s="62" t="s">
         <v>165</v>
       </c>
-      <c r="H26" s="64"/>
-      <c r="I26" s="59"/>
-    </row>
-    <row r="27" spans="1:9" s="55" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A27" s="63"/>
-      <c r="B27" s="64"/>
-      <c r="C27" s="58" t="s">
+      <c r="H26" s="62"/>
+      <c r="I26" s="57" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A27" s="61"/>
+      <c r="B27" s="62"/>
+      <c r="C27" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D27" s="58" t="s">
+      <c r="D27" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="E27" s="59" t="s">
+      <c r="E27" s="57" t="s">
         <v>168</v>
       </c>
-      <c r="F27" s="59"/>
-      <c r="G27" s="64" t="s">
+      <c r="F27" s="57"/>
+      <c r="G27" s="62" t="s">
         <v>165</v>
       </c>
-      <c r="H27" s="64"/>
-      <c r="I27" s="59"/>
-    </row>
-    <row r="28" spans="1:9" s="55" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A28" s="63"/>
-      <c r="B28" s="64"/>
-      <c r="C28" s="58" t="s">
+      <c r="H27" s="62"/>
+      <c r="I27" s="57"/>
+    </row>
+    <row r="28" spans="1:9" s="53" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A28" s="61"/>
+      <c r="B28" s="62"/>
+      <c r="C28" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D28" s="58" t="s">
+      <c r="D28" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="E28" s="59" t="s">
+      <c r="E28" s="57" t="s">
         <v>171</v>
       </c>
-      <c r="F28" s="59"/>
-      <c r="G28" s="64" t="s">
+      <c r="F28" s="57"/>
+      <c r="G28" s="62" t="s">
         <v>165</v>
       </c>
-      <c r="H28" s="64"/>
-      <c r="I28" s="59"/>
-    </row>
-    <row r="29" spans="1:9" s="55" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A29" s="63"/>
-      <c r="B29" s="64"/>
-      <c r="C29" s="58" t="s">
+      <c r="H28" s="62"/>
+      <c r="I28" s="57"/>
+    </row>
+    <row r="29" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A29" s="61"/>
+      <c r="B29" s="62"/>
+      <c r="C29" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D29" s="58" t="s">
+      <c r="D29" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="E29" s="59" t="s">
+      <c r="E29" s="57" t="s">
         <v>169</v>
       </c>
-      <c r="F29" s="59"/>
-      <c r="G29" s="64" t="s">
+      <c r="F29" s="57"/>
+      <c r="G29" s="62" t="s">
         <v>165</v>
       </c>
-      <c r="H29" s="64"/>
-      <c r="I29" s="59"/>
-    </row>
-    <row r="30" spans="1:9" s="55" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A30" s="63"/>
-      <c r="B30" s="64"/>
-      <c r="C30" s="58" t="s">
+      <c r="H29" s="62"/>
+      <c r="I29" s="57"/>
+    </row>
+    <row r="30" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A30" s="61"/>
+      <c r="B30" s="62"/>
+      <c r="C30" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D30" s="58" t="s">
+      <c r="D30" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="E30" s="59" t="s">
+      <c r="E30" s="57" t="s">
         <v>172</v>
       </c>
-      <c r="F30" s="59"/>
-      <c r="G30" s="64" t="s">
+      <c r="F30" s="57"/>
+      <c r="G30" s="62" t="s">
         <v>165</v>
       </c>
-      <c r="H30" s="64"/>
-      <c r="I30" s="59"/>
-    </row>
-    <row r="31" spans="1:9" s="55" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A31" s="51">
+      <c r="H30" s="62"/>
+      <c r="I30" s="57"/>
+    </row>
+    <row r="31" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A31" s="49">
         <v>2</v>
       </c>
-      <c r="B31" s="52">
+      <c r="B31" s="50">
         <v>2</v>
       </c>
-      <c r="C31" s="53" t="s">
+      <c r="C31" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="D31" s="53" t="s">
+      <c r="D31" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="E31" s="54" t="s">
+      <c r="E31" s="52" t="s">
         <v>154</v>
       </c>
-      <c r="F31" s="54"/>
-      <c r="G31" s="52"/>
-      <c r="H31" s="52" t="s">
+      <c r="F31" s="52"/>
+      <c r="G31" s="50"/>
+      <c r="H31" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I31" s="53" t="s">
+      <c r="I31" s="51" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:9" s="55" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A32" s="63"/>
-      <c r="B32" s="64"/>
-      <c r="C32" s="58" t="s">
+    <row r="32" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A32" s="61"/>
+      <c r="B32" s="62"/>
+      <c r="C32" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D32" s="58" t="s">
+      <c r="D32" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="E32" s="59" t="s">
+      <c r="E32" s="57" t="s">
         <v>177</v>
       </c>
-      <c r="F32" s="59"/>
-      <c r="G32" s="64" t="s">
+      <c r="F32" s="57"/>
+      <c r="G32" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="H32" s="64"/>
-      <c r="I32" s="59"/>
-    </row>
-    <row r="33" spans="1:9" s="55" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A33" s="63"/>
-      <c r="B33" s="64"/>
-      <c r="C33" s="58" t="s">
+      <c r="H32" s="62"/>
+      <c r="I32" s="57"/>
+    </row>
+    <row r="33" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A33" s="61"/>
+      <c r="B33" s="62"/>
+      <c r="C33" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D33" s="58" t="s">
+      <c r="D33" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="E33" s="59" t="s">
+      <c r="E33" s="57" t="s">
         <v>186</v>
       </c>
-      <c r="F33" s="59"/>
-      <c r="G33" s="64" t="s">
+      <c r="F33" s="57"/>
+      <c r="G33" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="H33" s="64"/>
-      <c r="I33" s="59"/>
-    </row>
-    <row r="34" spans="1:9" s="55" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A34" s="63"/>
-      <c r="B34" s="64"/>
-      <c r="C34" s="58" t="s">
+      <c r="H33" s="62"/>
+      <c r="I33" s="57"/>
+    </row>
+    <row r="34" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A34" s="61"/>
+      <c r="B34" s="62"/>
+      <c r="C34" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D34" s="58" t="s">
+      <c r="D34" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="E34" s="59" t="s">
+      <c r="E34" s="57" t="s">
         <v>187</v>
       </c>
-      <c r="F34" s="59"/>
-      <c r="G34" s="64"/>
-      <c r="H34" s="64"/>
-      <c r="I34" s="59"/>
-    </row>
-    <row r="35" spans="1:9" s="55" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A35" s="63"/>
-      <c r="B35" s="64"/>
-      <c r="C35" s="58" t="s">
+      <c r="F34" s="57"/>
+      <c r="G34" s="62"/>
+      <c r="H34" s="62"/>
+      <c r="I34" s="57"/>
+    </row>
+    <row r="35" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A35" s="61"/>
+      <c r="B35" s="62"/>
+      <c r="C35" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D35" s="58" t="s">
+      <c r="D35" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="E35" s="59" t="s">
+      <c r="E35" s="57" t="s">
         <v>162</v>
       </c>
-      <c r="F35" s="59"/>
-      <c r="G35" s="64" t="s">
+      <c r="F35" s="57"/>
+      <c r="G35" s="62" t="s">
         <v>201</v>
       </c>
-      <c r="H35" s="64"/>
-      <c r="I35" s="59"/>
-    </row>
-    <row r="36" spans="1:9" s="55" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A36" s="63"/>
-      <c r="B36" s="64"/>
-      <c r="C36" s="58" t="s">
+      <c r="H35" s="62"/>
+      <c r="I35" s="57"/>
+    </row>
+    <row r="36" spans="1:9" s="53" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A36" s="61"/>
+      <c r="B36" s="62"/>
+      <c r="C36" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D36" s="58" t="s">
+      <c r="D36" s="56" t="s">
         <v>157</v>
       </c>
-      <c r="E36" s="59" t="s">
+      <c r="E36" s="57" t="s">
         <v>159</v>
       </c>
-      <c r="F36" s="59"/>
-      <c r="G36" s="64" t="s">
+      <c r="F36" s="57"/>
+      <c r="G36" s="62" t="s">
         <v>201</v>
       </c>
-      <c r="H36" s="64"/>
-      <c r="I36" s="59"/>
-    </row>
-    <row r="37" spans="1:9" s="55" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A37" s="63"/>
-      <c r="B37" s="64"/>
-      <c r="C37" s="58" t="s">
+      <c r="H36" s="62"/>
+      <c r="I36" s="57"/>
+    </row>
+    <row r="37" spans="1:9" s="53" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A37" s="61"/>
+      <c r="B37" s="62"/>
+      <c r="C37" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D37" s="58" t="s">
+      <c r="D37" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="E37" s="59" t="s">
+      <c r="E37" s="57" t="s">
         <v>188</v>
       </c>
-      <c r="F37" s="59"/>
-      <c r="G37" s="64" t="s">
+      <c r="F37" s="57"/>
+      <c r="G37" s="62" t="s">
         <v>201</v>
       </c>
-      <c r="H37" s="64"/>
-      <c r="I37" s="59"/>
-    </row>
-    <row r="38" spans="1:9" s="55" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A38" s="63"/>
-      <c r="B38" s="64"/>
-      <c r="C38" s="58" t="s">
+      <c r="H37" s="62"/>
+      <c r="I37" s="57"/>
+    </row>
+    <row r="38" spans="1:9" s="53" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A38" s="61"/>
+      <c r="B38" s="62"/>
+      <c r="C38" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D38" s="58" t="s">
+      <c r="D38" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="E38" s="59" t="s">
+      <c r="E38" s="57" t="s">
         <v>160</v>
       </c>
-      <c r="F38" s="59"/>
-      <c r="G38" s="64" t="s">
+      <c r="F38" s="57"/>
+      <c r="G38" s="62" t="s">
         <v>201</v>
       </c>
-      <c r="H38" s="64"/>
-      <c r="I38" s="59"/>
-    </row>
-    <row r="39" spans="1:9" s="55" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A39" s="63"/>
-      <c r="B39" s="64"/>
-      <c r="C39" s="58" t="s">
+      <c r="H38" s="62"/>
+      <c r="I38" s="57"/>
+    </row>
+    <row r="39" spans="1:9" s="53" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A39" s="61"/>
+      <c r="B39" s="62"/>
+      <c r="C39" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D39" s="58" t="s">
+      <c r="D39" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="E39" s="59" t="s">
+      <c r="E39" s="57" t="s">
         <v>161</v>
       </c>
-      <c r="F39" s="59"/>
-      <c r="G39" s="64" t="s">
+      <c r="F39" s="57"/>
+      <c r="G39" s="62" t="s">
         <v>201</v>
       </c>
-      <c r="H39" s="64"/>
-      <c r="I39" s="59"/>
-    </row>
-    <row r="40" spans="1:9" s="55" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A40" s="63"/>
-      <c r="B40" s="64"/>
-      <c r="C40" s="58" t="s">
+      <c r="H39" s="62"/>
+      <c r="I39" s="57"/>
+    </row>
+    <row r="40" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A40" s="61"/>
+      <c r="B40" s="62"/>
+      <c r="C40" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D40" s="58" t="s">
+      <c r="D40" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="E40" s="59" t="s">
+      <c r="E40" s="57" t="s">
         <v>172</v>
       </c>
-      <c r="F40" s="59"/>
-      <c r="G40" s="64" t="s">
+      <c r="F40" s="57"/>
+      <c r="G40" s="62" t="s">
         <v>201</v>
       </c>
-      <c r="H40" s="64"/>
-      <c r="I40" s="59"/>
-    </row>
-    <row r="41" spans="1:9" s="55" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A41" s="63"/>
-      <c r="B41" s="64"/>
-      <c r="C41" s="58" t="s">
+      <c r="H40" s="62"/>
+      <c r="I40" s="57"/>
+    </row>
+    <row r="41" spans="1:9" s="53" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A41" s="61"/>
+      <c r="B41" s="62"/>
+      <c r="C41" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D41" s="58" t="s">
+      <c r="D41" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="E41" s="59" t="s">
+      <c r="E41" s="57" t="s">
         <v>158</v>
       </c>
-      <c r="F41" s="59"/>
-      <c r="G41" s="64" t="s">
+      <c r="F41" s="57"/>
+      <c r="G41" s="62" t="s">
         <v>201</v>
       </c>
-      <c r="H41" s="64"/>
-      <c r="I41" s="59"/>
-    </row>
-    <row r="42" spans="1:9" s="55" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A42" s="63"/>
-      <c r="B42" s="64"/>
-      <c r="C42" s="58" t="s">
+      <c r="H41" s="62"/>
+      <c r="I41" s="57"/>
+    </row>
+    <row r="42" spans="1:9" s="53" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A42" s="61"/>
+      <c r="B42" s="62"/>
+      <c r="C42" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D42" s="58" t="s">
+      <c r="D42" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="E42" s="59" t="s">
+      <c r="E42" s="57" t="s">
         <v>171</v>
       </c>
-      <c r="F42" s="59"/>
-      <c r="G42" s="64" t="s">
+      <c r="F42" s="57"/>
+      <c r="G42" s="62" t="s">
         <v>201</v>
       </c>
-      <c r="H42" s="64"/>
-      <c r="I42" s="59"/>
-    </row>
-    <row r="43" spans="1:9" s="55" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A43" s="56"/>
-      <c r="B43" s="57"/>
-      <c r="C43" s="58" t="s">
+      <c r="H42" s="62"/>
+      <c r="I42" s="57"/>
+    </row>
+    <row r="43" spans="1:9" s="53" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A43" s="54"/>
+      <c r="B43" s="55"/>
+      <c r="C43" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D43" s="58" t="s">
+      <c r="D43" s="56" t="s">
         <v>200</v>
       </c>
-      <c r="E43" s="59" t="s">
+      <c r="E43" s="57" t="s">
         <v>199</v>
       </c>
-      <c r="F43" s="60"/>
-      <c r="G43" s="64" t="s">
+      <c r="F43" s="58"/>
+      <c r="G43" s="62" t="s">
         <v>201</v>
       </c>
-      <c r="H43" s="61"/>
-      <c r="I43" s="62"/>
-    </row>
-    <row r="44" spans="1:9" s="55" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A44" s="63"/>
-      <c r="B44" s="64"/>
-      <c r="C44" s="58" t="s">
+      <c r="H43" s="59"/>
+      <c r="I43" s="60"/>
+    </row>
+    <row r="44" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A44" s="61"/>
+      <c r="B44" s="62"/>
+      <c r="C44" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="D44" s="58" t="s">
+      <c r="D44" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="E44" s="59" t="s">
+      <c r="E44" s="57" t="s">
         <v>152</v>
       </c>
-      <c r="F44" s="59"/>
-      <c r="G44" s="64" t="s">
+      <c r="F44" s="57"/>
+      <c r="G44" s="62" t="s">
         <v>201</v>
       </c>
-      <c r="H44" s="64"/>
-      <c r="I44" s="59"/>
-    </row>
-    <row r="45" spans="1:9" s="55" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A45" s="51">
+      <c r="H44" s="62"/>
+      <c r="I44" s="57"/>
+    </row>
+    <row r="45" spans="1:9" s="53" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A45" s="49">
         <v>2</v>
       </c>
-      <c r="B45" s="52">
+      <c r="B45" s="50">
         <v>3</v>
       </c>
-      <c r="C45" s="53" t="s">
+      <c r="C45" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="D45" s="53" t="s">
+      <c r="D45" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="E45" s="54" t="s">
+      <c r="E45" s="52" t="s">
         <v>150</v>
       </c>
-      <c r="F45" s="54"/>
-      <c r="G45" s="52"/>
-      <c r="H45" s="52" t="s">
+      <c r="F45" s="52"/>
+      <c r="G45" s="50"/>
+      <c r="H45" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="53" t="s">
+      <c r="I45" s="51" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:9" s="55" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A46" s="63"/>
-      <c r="B46" s="64"/>
-      <c r="C46" s="58"/>
-      <c r="D46" s="58" t="s">
+    <row r="46" spans="1:9" s="53" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A46" s="61"/>
+      <c r="B46" s="62"/>
+      <c r="C46" s="56"/>
+      <c r="D46" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="E46" s="59" t="s">
+      <c r="E46" s="57" t="s">
         <v>193</v>
       </c>
-      <c r="F46" s="59"/>
-      <c r="G46" s="64"/>
-      <c r="H46" s="64"/>
-      <c r="I46" s="58"/>
-    </row>
-    <row r="47" spans="1:9" s="55" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A47" s="63"/>
-      <c r="B47" s="64"/>
-      <c r="C47" s="58"/>
-      <c r="D47" s="58" t="s">
+      <c r="F46" s="57"/>
+      <c r="G46" s="62"/>
+      <c r="H46" s="62"/>
+      <c r="I46" s="56"/>
+    </row>
+    <row r="47" spans="1:9" s="53" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A47" s="61"/>
+      <c r="B47" s="62"/>
+      <c r="C47" s="56"/>
+      <c r="D47" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="E47" s="59" t="s">
+      <c r="E47" s="57" t="s">
         <v>189</v>
       </c>
-      <c r="F47" s="59"/>
-      <c r="G47" s="64"/>
-      <c r="H47" s="64"/>
-      <c r="I47" s="58"/>
-    </row>
-    <row r="48" spans="1:9" s="55" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A48" s="63"/>
-      <c r="B48" s="64"/>
-      <c r="C48" s="58"/>
-      <c r="D48" s="58" t="s">
+      <c r="F47" s="57"/>
+      <c r="G47" s="62"/>
+      <c r="H47" s="62"/>
+      <c r="I47" s="56"/>
+    </row>
+    <row r="48" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A48" s="61"/>
+      <c r="B48" s="62"/>
+      <c r="C48" s="56"/>
+      <c r="D48" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="E48" s="59" t="s">
+      <c r="E48" s="57" t="s">
         <v>191</v>
       </c>
-      <c r="F48" s="59"/>
-      <c r="G48" s="64"/>
-      <c r="H48" s="64"/>
-      <c r="I48" s="58"/>
-    </row>
-    <row r="49" spans="1:9" s="55" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A49" s="63"/>
-      <c r="B49" s="64"/>
-      <c r="C49" s="58"/>
-      <c r="D49" s="58" t="s">
+      <c r="F48" s="57"/>
+      <c r="G48" s="62"/>
+      <c r="H48" s="62"/>
+      <c r="I48" s="56"/>
+    </row>
+    <row r="49" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A49" s="61"/>
+      <c r="B49" s="62"/>
+      <c r="C49" s="56"/>
+      <c r="D49" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="E49" s="59" t="s">
+      <c r="E49" s="57" t="s">
         <v>192</v>
       </c>
-      <c r="F49" s="59"/>
-      <c r="G49" s="64"/>
-      <c r="H49" s="64"/>
-      <c r="I49" s="58"/>
-    </row>
-    <row r="50" spans="1:9" s="55" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A50" s="63"/>
-      <c r="B50" s="64"/>
-      <c r="C50" s="58"/>
-      <c r="D50" s="58" t="s">
+      <c r="F49" s="57"/>
+      <c r="G49" s="62"/>
+      <c r="H49" s="62"/>
+      <c r="I49" s="56"/>
+    </row>
+    <row r="50" spans="1:9" s="53" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A50" s="61"/>
+      <c r="B50" s="62"/>
+      <c r="C50" s="56"/>
+      <c r="D50" s="56" t="s">
         <v>157</v>
       </c>
-      <c r="E50" s="59" t="s">
+      <c r="E50" s="57" t="s">
         <v>190</v>
       </c>
-      <c r="F50" s="59"/>
-      <c r="G50" s="64"/>
-      <c r="H50" s="64"/>
-      <c r="I50" s="58"/>
+      <c r="F50" s="57"/>
+      <c r="G50" s="62"/>
+      <c r="H50" s="62"/>
+      <c r="I50" s="56"/>
     </row>
     <row r="51" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="10"/>
@@ -13769,17 +13781,17 @@
       <c r="I32" s="12"/>
     </row>
     <row r="33" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A33" s="49" t="s">
+      <c r="A33" s="63" t="s">
         <v>103</v>
       </c>
-      <c r="B33" s="50"/>
-      <c r="C33" s="50"/>
-      <c r="D33" s="50"/>
-      <c r="E33" s="50"/>
-      <c r="F33" s="50"/>
-      <c r="G33" s="50"/>
-      <c r="H33" s="50"/>
-      <c r="I33" s="50"/>
+      <c r="B33" s="64"/>
+      <c r="C33" s="64"/>
+      <c r="D33" s="64"/>
+      <c r="E33" s="64"/>
+      <c r="F33" s="64"/>
+      <c r="G33" s="64"/>
+      <c r="H33" s="64"/>
+      <c r="I33" s="64"/>
     </row>
     <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="10"/>
@@ -25114,17 +25126,17 @@
       <c r="I18" s="12"/>
     </row>
     <row r="19" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A19" s="49" t="s">
+      <c r="A19" s="63" t="s">
         <v>103</v>
       </c>
-      <c r="B19" s="50"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="50"/>
-      <c r="H19" s="50"/>
-      <c r="I19" s="50"/>
+      <c r="B19" s="64"/>
+      <c r="C19" s="64"/>
+      <c r="D19" s="64"/>
+      <c r="E19" s="64"/>
+      <c r="F19" s="64"/>
+      <c r="G19" s="64"/>
+      <c r="H19" s="64"/>
+      <c r="I19" s="64"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>

</xml_diff>

<commit_message>
Rose - added new test for SupplierLogin
</commit_message>
<xml_diff>
--- a/OfficialInternalBacklog.xlsx
+++ b/OfficialInternalBacklog.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pat B\Capstone-2015\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" tabRatio="291"/>
   </bookViews>
@@ -24,7 +19,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BacklogSprint3!$A$1:$I$1</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">BacklogSprint1!$A$1:$I$41</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">BacklogSprint2!$A$1:$I$53</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">BacklogSprint3!$A$1:$I$60</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">BacklogSprint3!$A$1:$I$62</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">BacklogSprint1!$1:$1</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">BacklogSprint2!$1:$1</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">BacklogSprint3!$1:$1</definedName>
@@ -34,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="285">
   <si>
     <t>Sprint</t>
   </si>
@@ -905,6 +900,12 @@
   <si>
     <t>Add Search Box to each tab in main window</t>
   </si>
+  <si>
+    <t>SupplierLogin Manager Methods</t>
+  </si>
+  <si>
+    <t>SupplierLogin Accessor Methods</t>
+  </si>
 </sst>
 </file>
 
@@ -1100,7 +1101,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1326,6 +1327,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1603,7 +1605,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1611,11 +1613,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1026"/>
+  <dimension ref="A1:I1028"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J48" sqref="J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1701,7 +1703,9 @@
         <v>18</v>
       </c>
       <c r="H3" s="61"/>
-      <c r="I3" s="87"/>
+      <c r="I3" s="87" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="4" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="60"/>
@@ -1722,7 +1726,9 @@
         <v>18</v>
       </c>
       <c r="H4" s="61"/>
-      <c r="I4" s="87"/>
+      <c r="I4" s="87" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
@@ -1741,7 +1747,9 @@
         <v>18</v>
       </c>
       <c r="H5" s="11"/>
-      <c r="I5" s="61"/>
+      <c r="I5" s="61" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
@@ -1760,7 +1768,9 @@
         <v>18</v>
       </c>
       <c r="H6" s="11"/>
-      <c r="I6" s="61"/>
+      <c r="I6" s="61" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
@@ -1779,7 +1789,9 @@
         <v>18</v>
       </c>
       <c r="H7" s="11"/>
-      <c r="I7" s="61"/>
+      <c r="I7" s="61" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="8" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A8" s="50">
@@ -2293,9 +2305,7 @@
         <v>275</v>
       </c>
       <c r="F36" s="14"/>
-      <c r="G36" s="61" t="s">
-        <v>18</v>
-      </c>
+      <c r="G36" s="61"/>
       <c r="H36" s="11"/>
       <c r="I36" s="61"/>
     </row>
@@ -2437,15 +2447,15 @@
       <c r="H44" s="11"/>
       <c r="I44" s="61"/>
     </row>
-    <row r="45" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" s="89" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
       <c r="B45" s="11"/>
       <c r="C45" s="11"/>
       <c r="D45" s="12" t="s">
-        <v>40</v>
+        <v>270</v>
       </c>
       <c r="E45" s="14" t="s">
-        <v>240</v>
+        <v>283</v>
       </c>
       <c r="F45" s="14" t="s">
         <v>237</v>
@@ -2454,23 +2464,25 @@
         <v>18</v>
       </c>
       <c r="H45" s="11"/>
-      <c r="I45" s="61"/>
-    </row>
-    <row r="46" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="I45" s="61" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="10"/>
       <c r="B46" s="11"/>
       <c r="C46" s="11"/>
-      <c r="D46" s="57" t="s">
-        <v>32</v>
-      </c>
-      <c r="E46" s="57" t="s">
-        <v>241</v>
+      <c r="D46" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E46" s="14" t="s">
+        <v>240</v>
       </c>
       <c r="F46" s="14" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="G46" s="61" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="H46" s="11"/>
       <c r="I46" s="61"/>
@@ -2483,12 +2495,14 @@
         <v>32</v>
       </c>
       <c r="E47" s="57" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F47" s="14" t="s">
         <v>242</v>
       </c>
-      <c r="G47" s="61"/>
+      <c r="G47" s="61" t="s">
+        <v>63</v>
+      </c>
       <c r="H47" s="11"/>
       <c r="I47" s="61"/>
     </row>
@@ -2500,18 +2514,16 @@
         <v>32</v>
       </c>
       <c r="E48" s="57" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F48" s="14" t="s">
         <v>242</v>
       </c>
-      <c r="G48" s="61" t="s">
-        <v>63</v>
-      </c>
+      <c r="G48" s="61"/>
       <c r="H48" s="11"/>
       <c r="I48" s="61"/>
     </row>
-    <row r="49" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" s="89" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="10"/>
       <c r="B49" s="11"/>
       <c r="C49" s="11"/>
@@ -2519,7 +2531,7 @@
         <v>32</v>
       </c>
       <c r="E49" s="57" t="s">
-        <v>245</v>
+        <v>284</v>
       </c>
       <c r="F49" s="14" t="s">
         <v>242</v>
@@ -2528,64 +2540,70 @@
         <v>18</v>
       </c>
       <c r="H49" s="11"/>
-      <c r="I49" s="61"/>
-    </row>
-    <row r="50" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A50" s="50">
-        <v>3</v>
-      </c>
-      <c r="B50" s="50">
-        <v>9</v>
-      </c>
-      <c r="C50" s="50" t="s">
-        <v>9</v>
-      </c>
-      <c r="D50" s="51" t="s">
-        <v>199</v>
-      </c>
-      <c r="E50" s="52" t="s">
-        <v>277</v>
-      </c>
-      <c r="F50" s="52"/>
-      <c r="G50" s="50"/>
-      <c r="H50" s="50"/>
-      <c r="I50" s="50" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="I49" s="61" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="10"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="57" t="s">
+        <v>32</v>
+      </c>
+      <c r="E50" s="57" t="s">
+        <v>244</v>
+      </c>
+      <c r="F50" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="G50" s="61" t="s">
+        <v>63</v>
+      </c>
+      <c r="H50" s="11"/>
+      <c r="I50" s="61"/>
+    </row>
+    <row r="51" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="10"/>
       <c r="B51" s="11"/>
       <c r="C51" s="11"/>
       <c r="D51" s="57" t="s">
-        <v>276</v>
+        <v>32</v>
       </c>
       <c r="E51" s="57" t="s">
-        <v>246</v>
-      </c>
-      <c r="F51" s="14"/>
+        <v>245</v>
+      </c>
+      <c r="F51" s="14" t="s">
+        <v>242</v>
+      </c>
       <c r="G51" s="61" t="s">
-        <v>72</v>
+        <v>18</v>
       </c>
       <c r="H51" s="11"/>
       <c r="I51" s="61"/>
     </row>
-    <row r="52" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A52" s="10"/>
-      <c r="B52" s="11"/>
-      <c r="C52" s="11"/>
-      <c r="D52" s="57" t="s">
-        <v>276</v>
-      </c>
-      <c r="E52" s="57" t="s">
-        <v>247</v>
-      </c>
-      <c r="F52" s="14"/>
-      <c r="G52" s="61" t="s">
-        <v>72</v>
-      </c>
-      <c r="H52" s="11"/>
-      <c r="I52" s="61"/>
+    <row r="52" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A52" s="50">
+        <v>3</v>
+      </c>
+      <c r="B52" s="50">
+        <v>9</v>
+      </c>
+      <c r="C52" s="50" t="s">
+        <v>9</v>
+      </c>
+      <c r="D52" s="51" t="s">
+        <v>199</v>
+      </c>
+      <c r="E52" s="52" t="s">
+        <v>277</v>
+      </c>
+      <c r="F52" s="52"/>
+      <c r="G52" s="50"/>
+      <c r="H52" s="50"/>
+      <c r="I52" s="50" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="53" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A53" s="10"/>
@@ -2595,7 +2613,7 @@
         <v>276</v>
       </c>
       <c r="E53" s="57" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F53" s="14"/>
       <c r="G53" s="61" t="s">
@@ -2612,7 +2630,7 @@
         <v>276</v>
       </c>
       <c r="E54" s="57" t="s">
-        <v>57</v>
+        <v>247</v>
       </c>
       <c r="F54" s="14"/>
       <c r="G54" s="61" t="s">
@@ -2621,58 +2639,62 @@
       <c r="H54" s="11"/>
       <c r="I54" s="61"/>
     </row>
-    <row r="55" spans="1:9" s="53" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A55" s="50">
-        <v>3</v>
-      </c>
-      <c r="B55" s="50">
-        <v>10</v>
-      </c>
-      <c r="C55" s="50" t="s">
-        <v>9</v>
-      </c>
-      <c r="D55" s="51" t="s">
-        <v>199</v>
-      </c>
-      <c r="E55" s="52" t="s">
-        <v>249</v>
-      </c>
-      <c r="F55" s="52"/>
-      <c r="G55" s="50"/>
-      <c r="H55" s="50"/>
-      <c r="I55" s="50" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A55" s="10"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="57" t="s">
+        <v>276</v>
+      </c>
+      <c r="E55" s="57" t="s">
+        <v>248</v>
+      </c>
+      <c r="F55" s="14"/>
+      <c r="G55" s="61" t="s">
+        <v>72</v>
+      </c>
+      <c r="H55" s="11"/>
+      <c r="I55" s="61"/>
+    </row>
+    <row r="56" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A56" s="10"/>
       <c r="B56" s="11"/>
       <c r="C56" s="11"/>
-      <c r="D56" s="12"/>
-      <c r="E56" s="14" t="s">
-        <v>280</v>
+      <c r="D56" s="57" t="s">
+        <v>276</v>
+      </c>
+      <c r="E56" s="57" t="s">
+        <v>57</v>
       </c>
       <c r="F56" s="14"/>
       <c r="G56" s="61" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="H56" s="11"/>
       <c r="I56" s="61"/>
     </row>
-    <row r="57" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="10"/>
-      <c r="B57" s="11"/>
-      <c r="C57" s="11"/>
-      <c r="D57" s="12"/>
-      <c r="E57" s="14" t="s">
-        <v>281</v>
-      </c>
-      <c r="F57" s="14"/>
-      <c r="G57" s="61" t="s">
-        <v>69</v>
-      </c>
-      <c r="H57" s="11"/>
-      <c r="I57" s="61"/>
+    <row r="57" spans="1:9" s="53" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A57" s="50">
+        <v>3</v>
+      </c>
+      <c r="B57" s="50">
+        <v>10</v>
+      </c>
+      <c r="C57" s="50" t="s">
+        <v>9</v>
+      </c>
+      <c r="D57" s="51" t="s">
+        <v>199</v>
+      </c>
+      <c r="E57" s="52" t="s">
+        <v>249</v>
+      </c>
+      <c r="F57" s="52"/>
+      <c r="G57" s="50"/>
+      <c r="H57" s="50"/>
+      <c r="I57" s="50" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="10"/>
@@ -2680,7 +2702,7 @@
       <c r="C58" s="11"/>
       <c r="D58" s="12"/>
       <c r="E58" s="14" t="s">
-        <v>250</v>
+        <v>280</v>
       </c>
       <c r="F58" s="14"/>
       <c r="G58" s="61" t="s">
@@ -2694,11 +2716,13 @@
       <c r="B59" s="11"/>
       <c r="C59" s="11"/>
       <c r="D59" s="12"/>
-      <c r="E59" s="88" t="s">
-        <v>282</v>
+      <c r="E59" s="14" t="s">
+        <v>281</v>
       </c>
       <c r="F59" s="14"/>
-      <c r="G59" s="61"/>
+      <c r="G59" s="61" t="s">
+        <v>69</v>
+      </c>
       <c r="H59" s="11"/>
       <c r="I59" s="61"/>
     </row>
@@ -2707,31 +2731,37 @@
       <c r="B60" s="11"/>
       <c r="C60" s="11"/>
       <c r="D60" s="12"/>
-      <c r="E60" s="88" t="s">
-        <v>224</v>
+      <c r="E60" s="14" t="s">
+        <v>250</v>
       </c>
       <c r="F60" s="14"/>
-      <c r="G60" s="61"/>
+      <c r="G60" s="61" t="s">
+        <v>69</v>
+      </c>
       <c r="H60" s="11"/>
       <c r="I60" s="61"/>
     </row>
-    <row r="61" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="10"/>
       <c r="B61" s="11"/>
       <c r="C61" s="11"/>
       <c r="D61" s="12"/>
-      <c r="E61" s="14"/>
+      <c r="E61" s="88" t="s">
+        <v>282</v>
+      </c>
       <c r="F61" s="14"/>
       <c r="G61" s="61"/>
       <c r="H61" s="11"/>
       <c r="I61" s="61"/>
     </row>
-    <row r="62" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="10"/>
       <c r="B62" s="11"/>
       <c r="C62" s="11"/>
       <c r="D62" s="12"/>
-      <c r="E62" s="14"/>
+      <c r="E62" s="88" t="s">
+        <v>224</v>
+      </c>
       <c r="F62" s="14"/>
       <c r="G62" s="61"/>
       <c r="H62" s="11"/>
@@ -13331,8 +13361,30 @@
       <c r="I1025" s="61"/>
     </row>
     <row r="1026" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1026" s="10"/>
+      <c r="B1026" s="11"/>
+      <c r="C1026" s="11"/>
       <c r="D1026" s="12"/>
       <c r="E1026" s="14"/>
+      <c r="F1026" s="14"/>
+      <c r="G1026" s="61"/>
+      <c r="H1026" s="11"/>
+      <c r="I1026" s="61"/>
+    </row>
+    <row r="1027" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1027" s="10"/>
+      <c r="B1027" s="11"/>
+      <c r="C1027" s="11"/>
+      <c r="D1027" s="12"/>
+      <c r="E1027" s="14"/>
+      <c r="F1027" s="14"/>
+      <c r="G1027" s="61"/>
+      <c r="H1027" s="11"/>
+      <c r="I1027" s="61"/>
+    </row>
+    <row r="1028" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="D1028" s="12"/>
+      <c r="E1028" s="14"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I1"/>
@@ -26099,17 +26151,17 @@
       <c r="I32" s="12"/>
     </row>
     <row r="33" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A33" s="89" t="s">
+      <c r="A33" s="90" t="s">
         <v>103</v>
       </c>
-      <c r="B33" s="90"/>
-      <c r="C33" s="90"/>
-      <c r="D33" s="90"/>
-      <c r="E33" s="90"/>
-      <c r="F33" s="90"/>
-      <c r="G33" s="90"/>
-      <c r="H33" s="90"/>
-      <c r="I33" s="90"/>
+      <c r="B33" s="91"/>
+      <c r="C33" s="91"/>
+      <c r="D33" s="91"/>
+      <c r="E33" s="91"/>
+      <c r="F33" s="91"/>
+      <c r="G33" s="91"/>
+      <c r="H33" s="91"/>
+      <c r="I33" s="91"/>
     </row>
     <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="10"/>
@@ -37444,17 +37496,17 @@
       <c r="I18" s="12"/>
     </row>
     <row r="19" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A19" s="89" t="s">
+      <c r="A19" s="90" t="s">
         <v>103</v>
       </c>
-      <c r="B19" s="90"/>
-      <c r="C19" s="90"/>
-      <c r="D19" s="90"/>
-      <c r="E19" s="90"/>
-      <c r="F19" s="90"/>
-      <c r="G19" s="90"/>
-      <c r="H19" s="90"/>
-      <c r="I19" s="90"/>
+      <c r="B19" s="91"/>
+      <c r="C19" s="91"/>
+      <c r="D19" s="91"/>
+      <c r="E19" s="91"/>
+      <c r="F19" s="91"/>
+      <c r="G19" s="91"/>
+      <c r="H19" s="91"/>
+      <c r="I19" s="91"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>

</xml_diff>

<commit_message>
Rose - test for HotelGuest
</commit_message>
<xml_diff>
--- a/OfficialInternalBacklog.xlsx
+++ b/OfficialInternalBacklog.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="285">
   <si>
     <t>Sprint</t>
   </si>
@@ -1605,7 +1605,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1616,8 +1616,8 @@
   <dimension ref="A1:I1028"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J48" sqref="J48"/>
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2424,7 +2424,9 @@
       <c r="F43" s="14" t="s">
         <v>237</v>
       </c>
-      <c r="G43" s="61"/>
+      <c r="G43" s="61" t="s">
+        <v>18</v>
+      </c>
       <c r="H43" s="11"/>
       <c r="I43" s="61"/>
     </row>
@@ -2485,7 +2487,9 @@
         <v>18</v>
       </c>
       <c r="H46" s="11"/>
-      <c r="I46" s="61"/>
+      <c r="I46" s="61" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
@@ -2519,7 +2523,9 @@
       <c r="F48" s="14" t="s">
         <v>242</v>
       </c>
-      <c r="G48" s="61"/>
+      <c r="G48" s="61" t="s">
+        <v>18</v>
+      </c>
       <c r="H48" s="11"/>
       <c r="I48" s="61"/>
     </row>
@@ -2580,7 +2586,9 @@
         <v>18</v>
       </c>
       <c r="H51" s="11"/>
-      <c r="I51" s="61"/>
+      <c r="I51" s="61" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="52" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A52" s="50">

</xml_diff>

<commit_message>
backlog update and checkout time
</commit_message>
<xml_diff>
--- a/OfficialInternalBacklog.xlsx
+++ b/OfficialInternalBacklog.xlsx
@@ -24,7 +24,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">BacklogSprint1!$A$1:$I$31</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">BacklogSprint2!$A$1:$I$20</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">BacklogSprint3!$A$1:$I$1</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">BacklogFinalSprint!$A$1:$I$35</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">BacklogFinalSprint!$A$1:$I$37</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">BacklogSprint1!$A$1:$I$41</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">BacklogSprint2!$A$1:$I$53</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">BacklogSprint3!$A$1:$I$53</definedName>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="355">
   <si>
     <t>Sprint</t>
   </si>
@@ -1025,9 +1025,6 @@
     <t>Matt</t>
   </si>
   <si>
-    <t>XML reports  for accounting and for each suppleir</t>
-  </si>
-  <si>
     <t>Printable report for suppliers to see their sales data</t>
   </si>
   <si>
@@ -1074,16 +1071,7 @@
     <t>Add confirmation box for guest booking</t>
   </si>
   <si>
-    <t>I agree to pay $x for the event xxx on xxx and charge to my credit card on file.</t>
-  </si>
-  <si>
     <t>Update the inserts to reflect accurate bookings so numbers match</t>
-  </si>
-  <si>
-    <t>Develop test cases and fill out to document the testing</t>
-  </si>
-  <si>
-    <t>Generate a random 5 digit pin for the guests</t>
   </si>
   <si>
     <t>Administrative control (WPF) for Event Types - Add/Edit/Archive</t>
@@ -1093,6 +1081,61 @@
   </si>
   <si>
     <t>If issue cannot be fixed in 5 min or less, file an issue on GitHub</t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>DONE
+4/24</t>
+  </si>
+  <si>
+    <t>Page for guest to view/print bookings</t>
+  </si>
+  <si>
+    <t>DONE 
+4/26</t>
+  </si>
+  <si>
+    <t>DONE 
+4/24</t>
+  </si>
+  <si>
+    <t>XML reports  for accounting and for each supplier</t>
+  </si>
+  <si>
+    <t>Rose
+Matt</t>
+  </si>
+  <si>
+    <t>80% done - probs with the date boxes and constraints = Kelsey/Arik can help</t>
+  </si>
+  <si>
+    <t>and searching is done   :)</t>
+  </si>
+  <si>
+    <t>item listing in business logic - presentation layer needs to check for result codes</t>
+  </si>
+  <si>
+    <t>I agree to pay $x for the event ___ on ___ and charge to my credit card on file.</t>
+  </si>
+  <si>
+    <t>Generate a random 6 digit pin for the guests</t>
+  </si>
+  <si>
+    <t>Website &amp; WPF</t>
+  </si>
+  <si>
+    <t>Perform User Testing</t>
+  </si>
+  <si>
+    <t>updated booking manage and fixed hotel guest and accessor  - will discuss strategy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moved stuff into test project </t>
+  </si>
+  <si>
+    <t>WCF Service</t>
   </si>
 </sst>
 </file>
@@ -1306,7 +1349,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1556,9 +1599,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1567,6 +1607,25 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1850,11 +1909,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1000"/>
+  <dimension ref="A1:I1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1923,7 +1982,7 @@
       <c r="A3" s="10"/>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
-      <c r="D3" s="102" t="s">
+      <c r="D3" s="101" t="s">
         <v>311</v>
       </c>
       <c r="E3" s="70" t="s">
@@ -1933,160 +1992,156 @@
       <c r="G3" s="68" t="s">
         <v>126</v>
       </c>
-      <c r="H3" s="61" t="s">
-        <v>321</v>
-      </c>
-      <c r="I3" s="61"/>
-    </row>
-    <row r="4" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A4" s="101"/>
-      <c r="B4" s="102"/>
-      <c r="C4" s="102"/>
-      <c r="D4" s="102" t="s">
+      <c r="H3" s="61"/>
+      <c r="I3" s="87" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="99" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="101" t="s">
+        <v>305</v>
+      </c>
+      <c r="E4" s="70" t="s">
+        <v>340</v>
+      </c>
+      <c r="F4" s="14"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="108" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A5" s="100"/>
+      <c r="B5" s="101"/>
+      <c r="C5" s="101"/>
+      <c r="D5" s="101" t="s">
         <v>311</v>
       </c>
-      <c r="E4" s="103" t="s">
-        <v>339</v>
-      </c>
-      <c r="F4" s="103"/>
-      <c r="G4" s="87" t="s">
+      <c r="E5" s="102" t="s">
+        <v>335</v>
+      </c>
+      <c r="F5" s="102"/>
+      <c r="G5" s="87" t="s">
         <v>307</v>
       </c>
-      <c r="H4" s="61" t="s">
-        <v>321</v>
-      </c>
-      <c r="I4" s="87"/>
-    </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.2">
-      <c r="A5" s="101"/>
-      <c r="B5" s="102"/>
-      <c r="C5" s="102"/>
-      <c r="D5" s="102" t="s">
+      <c r="H5" s="61"/>
+      <c r="I5" s="87" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+      <c r="A6" s="100"/>
+      <c r="B6" s="101"/>
+      <c r="C6" s="101"/>
+      <c r="D6" s="105" t="s">
         <v>312</v>
       </c>
-      <c r="E5" s="103" t="s">
+      <c r="E6" s="106" t="s">
+        <v>343</v>
+      </c>
+      <c r="F6" s="106"/>
+      <c r="G6" s="107" t="s">
+        <v>308</v>
+      </c>
+      <c r="H6" s="92"/>
+      <c r="I6" s="92"/>
+    </row>
+    <row r="7" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A7" s="100"/>
+      <c r="B7" s="101"/>
+      <c r="C7" s="101"/>
+      <c r="D7" s="105" t="s">
+        <v>305</v>
+      </c>
+      <c r="E7" s="106" t="s">
+        <v>296</v>
+      </c>
+      <c r="F7" s="106"/>
+      <c r="G7" s="107" t="s">
+        <v>344</v>
+      </c>
+      <c r="H7" s="61"/>
+      <c r="I7" s="87"/>
+    </row>
+    <row r="8" spans="1:9" s="53" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" s="100"/>
+      <c r="B8" s="101"/>
+      <c r="C8" s="101"/>
+      <c r="D8" s="105" t="s">
+        <v>311</v>
+      </c>
+      <c r="E8" s="106" t="s">
+        <v>354</v>
+      </c>
+      <c r="F8" s="106"/>
+      <c r="G8" s="107" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="61"/>
+      <c r="I8" s="87"/>
+    </row>
+    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+      <c r="A9" s="100"/>
+      <c r="B9" s="101"/>
+      <c r="C9" s="101"/>
+      <c r="D9" s="101" t="s">
+        <v>305</v>
+      </c>
+      <c r="E9" s="102" t="s">
+        <v>310</v>
+      </c>
+      <c r="F9" s="102"/>
+      <c r="G9" s="87" t="s">
+        <v>309</v>
+      </c>
+      <c r="H9" s="61"/>
+      <c r="I9" s="68" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A10" s="100"/>
+      <c r="B10" s="101"/>
+      <c r="C10" s="101"/>
+      <c r="D10" s="101" t="s">
+        <v>305</v>
+      </c>
+      <c r="E10" s="102" t="s">
         <v>319</v>
       </c>
-      <c r="F5" s="103"/>
-      <c r="G5" s="87" t="s">
-        <v>308</v>
-      </c>
-      <c r="H5" s="61" t="s">
-        <v>321</v>
-      </c>
-      <c r="I5" s="61"/>
-    </row>
-    <row r="6" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A6" s="101"/>
-      <c r="B6" s="102"/>
-      <c r="C6" s="102"/>
-      <c r="D6" s="102" t="s">
-        <v>305</v>
-      </c>
-      <c r="E6" s="103" t="s">
-        <v>296</v>
-      </c>
-      <c r="F6" s="103"/>
-      <c r="G6" s="87" t="s">
-        <v>318</v>
-      </c>
-      <c r="H6" s="61" t="s">
-        <v>321</v>
-      </c>
-      <c r="I6" s="87"/>
-    </row>
-    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.2">
-      <c r="A7" s="101"/>
-      <c r="B7" s="102"/>
-      <c r="C7" s="102"/>
-      <c r="D7" s="102" t="s">
-        <v>305</v>
-      </c>
-      <c r="E7" s="103" t="s">
-        <v>310</v>
-      </c>
-      <c r="F7" s="103"/>
-      <c r="G7" s="87" t="s">
+      <c r="F10" s="102"/>
+      <c r="G10" s="87" t="s">
         <v>309</v>
       </c>
-      <c r="H7" s="61" t="s">
-        <v>321</v>
-      </c>
-      <c r="I7" s="61"/>
-    </row>
-    <row r="8" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A8" s="101"/>
-      <c r="B8" s="102"/>
-      <c r="C8" s="102"/>
-      <c r="D8" s="102" t="s">
-        <v>305</v>
-      </c>
-      <c r="E8" s="103" t="s">
+      <c r="H10" s="61" t="s">
         <v>320</v>
       </c>
-      <c r="F8" s="103"/>
-      <c r="G8" s="87" t="s">
-        <v>309</v>
-      </c>
-      <c r="H8" s="61" t="s">
-        <v>321</v>
-      </c>
-      <c r="I8" s="61"/>
-    </row>
-    <row r="9" spans="1:9" s="53" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="50">
+      <c r="I10" s="68" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="53" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A11" s="50">
         <v>4</v>
       </c>
-      <c r="B9" s="50"/>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="52" t="s">
+      <c r="B11" s="50"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="52" t="s">
         <v>317</v>
       </c>
-      <c r="F9" s="52"/>
-      <c r="G9" s="50"/>
-      <c r="H9" s="50"/>
-      <c r="I9" s="50" t="s">
+      <c r="F11" s="52"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="50" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="57" t="s">
-        <v>305</v>
-      </c>
-      <c r="E10" s="57" t="s">
-        <v>326</v>
-      </c>
-      <c r="F10" s="14"/>
-      <c r="G10" s="87" t="s">
-        <v>318</v>
-      </c>
-      <c r="H10" s="11"/>
-      <c r="I10" s="61"/>
-    </row>
-    <row r="11" spans="1:9" s="98" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="57" t="s">
-        <v>305</v>
-      </c>
-      <c r="E11" s="57" t="s">
-        <v>327</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>328</v>
-      </c>
-      <c r="G11" s="87" t="s">
-        <v>318</v>
-      </c>
-      <c r="H11" s="11"/>
-      <c r="I11" s="61"/>
-    </row>
-    <row r="12" spans="1:9" s="98" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
@@ -2094,148 +2149,174 @@
         <v>305</v>
       </c>
       <c r="E12" s="57" t="s">
-        <v>329</v>
-      </c>
-      <c r="F12" s="14"/>
+        <v>325</v>
+      </c>
+      <c r="F12" s="88" t="s">
+        <v>345</v>
+      </c>
       <c r="G12" s="87" t="s">
         <v>318</v>
       </c>
       <c r="H12" s="11"/>
       <c r="I12" s="61"/>
     </row>
-    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" s="98" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
       <c r="D13" s="57" t="s">
-        <v>332</v>
+        <v>305</v>
       </c>
       <c r="E13" s="57" t="s">
-        <v>330</v>
-      </c>
-      <c r="F13" s="14"/>
+        <v>326</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>327</v>
+      </c>
       <c r="G13" s="87" t="s">
-        <v>126</v>
+        <v>318</v>
       </c>
       <c r="H13" s="11"/>
-      <c r="I13" s="61"/>
-    </row>
-    <row r="14" spans="1:9" s="98" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I13" s="68" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="98" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
       <c r="D14" s="57" t="s">
-        <v>332</v>
+        <v>305</v>
       </c>
       <c r="E14" s="57" t="s">
-        <v>331</v>
-      </c>
-      <c r="F14" s="14"/>
+        <v>328</v>
+      </c>
+      <c r="F14" s="88" t="s">
+        <v>346</v>
+      </c>
       <c r="G14" s="87" t="s">
-        <v>126</v>
+        <v>318</v>
       </c>
       <c r="H14" s="11"/>
-      <c r="I14" s="61"/>
-    </row>
-    <row r="15" spans="1:9" s="98" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="I14" s="68" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
       <c r="D15" s="57" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E15" s="57" t="s">
-        <v>334</v>
-      </c>
-      <c r="F15" s="103" t="s">
-        <v>335</v>
-      </c>
-      <c r="G15" s="87" t="s">
-        <v>126</v>
+        <v>329</v>
+      </c>
+      <c r="F15" s="88" t="s">
+        <v>347</v>
+      </c>
+      <c r="G15" s="108" t="s">
+        <v>318</v>
       </c>
       <c r="H15" s="11"/>
-      <c r="I15" s="61"/>
-    </row>
-    <row r="16" spans="1:9" s="98" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="I15" s="68" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="98" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
       <c r="D16" s="57" t="s">
-        <v>311</v>
+        <v>331</v>
       </c>
       <c r="E16" s="57" t="s">
-        <v>338</v>
-      </c>
-      <c r="F16" s="103"/>
+        <v>330</v>
+      </c>
+      <c r="F16" s="14"/>
       <c r="G16" s="87" t="s">
         <v>126</v>
       </c>
       <c r="H16" s="11"/>
-      <c r="I16" s="61"/>
+      <c r="I16" s="68" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="17" spans="1:9" s="98" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
       <c r="D17" s="57" t="s">
-        <v>311</v>
+        <v>332</v>
       </c>
       <c r="E17" s="57" t="s">
-        <v>336</v>
-      </c>
-      <c r="F17" s="103"/>
+        <v>333</v>
+      </c>
+      <c r="F17" s="109" t="s">
+        <v>348</v>
+      </c>
       <c r="G17" s="87" t="s">
         <v>126</v>
       </c>
       <c r="H17" s="11"/>
-      <c r="I17" s="61"/>
-    </row>
-    <row r="18" spans="1:9" s="53" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="50">
-        <v>4</v>
-      </c>
-      <c r="B18" s="50"/>
-      <c r="C18" s="51"/>
-      <c r="D18" s="51"/>
-      <c r="E18" s="52" t="s">
-        <v>298</v>
-      </c>
-      <c r="F18" s="52"/>
-      <c r="G18" s="50"/>
-      <c r="H18" s="50"/>
-      <c r="I18" s="50" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="I17" s="68" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="98" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="10"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="57" t="s">
+        <v>311</v>
+      </c>
+      <c r="E18" s="70" t="s">
+        <v>349</v>
+      </c>
+      <c r="F18" s="102"/>
+      <c r="G18" s="87" t="s">
+        <v>126</v>
+      </c>
+      <c r="H18" s="11"/>
+      <c r="I18" s="68" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="98" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
-      <c r="D19" s="57"/>
+      <c r="D19" s="57" t="s">
+        <v>311</v>
+      </c>
       <c r="E19" s="57" t="s">
-        <v>299</v>
-      </c>
-      <c r="F19" s="14"/>
+        <v>334</v>
+      </c>
+      <c r="F19" s="102"/>
       <c r="G19" s="87" t="s">
-        <v>313</v>
+        <v>126</v>
       </c>
       <c r="H19" s="11"/>
-      <c r="I19" s="61"/>
-    </row>
-    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="57"/>
-      <c r="E20" s="57" t="s">
-        <v>322</v>
-      </c>
-      <c r="F20" s="14"/>
-      <c r="G20" s="87" t="s">
-        <v>313</v>
-      </c>
-      <c r="H20" s="11"/>
-      <c r="I20" s="61"/>
+      <c r="I19" s="68" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="53" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A20" s="50">
+        <v>4</v>
+      </c>
+      <c r="B20" s="50"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="52" t="s">
+        <v>298</v>
+      </c>
+      <c r="F20" s="52"/>
+      <c r="G20" s="50"/>
+      <c r="H20" s="50"/>
+      <c r="I20" s="50" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
@@ -2243,7 +2324,7 @@
       <c r="C21" s="11"/>
       <c r="D21" s="57"/>
       <c r="E21" s="57" t="s">
-        <v>340</v>
+        <v>299</v>
       </c>
       <c r="F21" s="14"/>
       <c r="G21" s="87" t="s">
@@ -2256,89 +2337,81 @@
       <c r="A22" s="10"/>
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
-      <c r="D22" s="90"/>
+      <c r="D22" s="57"/>
       <c r="E22" s="57" t="s">
-        <v>300</v>
-      </c>
-      <c r="F22" s="91"/>
+        <v>321</v>
+      </c>
+      <c r="F22" s="14"/>
       <c r="G22" s="87" t="s">
         <v>313</v>
       </c>
       <c r="H22" s="11"/>
       <c r="I22" s="61"/>
     </row>
-    <row r="23" spans="1:9" s="53" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A23" s="50"/>
-      <c r="B23" s="50"/>
-      <c r="C23" s="50" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" s="51" t="s">
-        <v>199</v>
-      </c>
-      <c r="E23" s="52" t="s">
-        <v>304</v>
-      </c>
-      <c r="F23" s="52"/>
-      <c r="G23" s="50"/>
-      <c r="H23" s="50"/>
-      <c r="I23" s="50" t="s">
-        <v>13</v>
-      </c>
+    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="10"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="57" t="s">
+        <v>336</v>
+      </c>
+      <c r="F23" s="14"/>
+      <c r="G23" s="87" t="s">
+        <v>313</v>
+      </c>
+      <c r="H23" s="11"/>
+      <c r="I23" s="61"/>
     </row>
     <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
-      <c r="D24" s="57" t="s">
-        <v>305</v>
-      </c>
+      <c r="D24" s="90"/>
       <c r="E24" s="57" t="s">
-        <v>337</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>341</v>
-      </c>
-      <c r="G24" s="68" t="s">
-        <v>306</v>
+        <v>300</v>
+      </c>
+      <c r="F24" s="91"/>
+      <c r="G24" s="87" t="s">
+        <v>313</v>
       </c>
       <c r="H24" s="11"/>
       <c r="I24" s="61"/>
     </row>
-    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="57" t="s">
-        <v>314</v>
-      </c>
-      <c r="E25" s="57" t="s">
-        <v>337</v>
-      </c>
-      <c r="F25" s="14" t="s">
-        <v>341</v>
-      </c>
-      <c r="G25" s="68" t="s">
-        <v>72</v>
-      </c>
-      <c r="H25" s="11"/>
-      <c r="I25" s="61"/>
+    <row r="25" spans="1:9" s="53" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A25" s="50"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="50" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="51" t="s">
+        <v>199</v>
+      </c>
+      <c r="E25" s="52" t="s">
+        <v>304</v>
+      </c>
+      <c r="F25" s="52"/>
+      <c r="G25" s="50"/>
+      <c r="H25" s="50"/>
+      <c r="I25" s="50" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
-      <c r="D26" s="57" t="s">
-        <v>305</v>
-      </c>
-      <c r="E26" s="57" t="s">
+      <c r="D26" s="70" t="s">
+        <v>350</v>
+      </c>
+      <c r="E26" s="70" t="s">
+        <v>351</v>
+      </c>
+      <c r="F26" s="14" t="s">
         <v>337</v>
       </c>
-      <c r="F26" s="14" t="s">
-        <v>341</v>
-      </c>
-      <c r="G26" s="85" t="s">
-        <v>316</v>
+      <c r="G26" s="68" t="s">
+        <v>306</v>
       </c>
       <c r="H26" s="11"/>
       <c r="I26" s="61"/>
@@ -2347,17 +2420,17 @@
       <c r="A27" s="10"/>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
-      <c r="D27" s="57" t="s">
-        <v>314</v>
-      </c>
-      <c r="E27" s="57" t="s">
+      <c r="D27" s="70" t="s">
+        <v>350</v>
+      </c>
+      <c r="E27" s="70" t="s">
+        <v>351</v>
+      </c>
+      <c r="F27" s="14" t="s">
         <v>337</v>
       </c>
-      <c r="F27" s="14" t="s">
-        <v>341</v>
-      </c>
-      <c r="G27" s="61" t="s">
-        <v>16</v>
+      <c r="G27" s="68" t="s">
+        <v>72</v>
       </c>
       <c r="H27" s="11"/>
       <c r="I27" s="61"/>
@@ -2366,147 +2439,167 @@
       <c r="A28" s="10"/>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
-      <c r="D28" s="57" t="s">
-        <v>305</v>
-      </c>
-      <c r="E28" s="57" t="s">
-        <v>323</v>
-      </c>
-      <c r="F28" s="14"/>
-      <c r="G28" s="61" t="s">
-        <v>318</v>
+      <c r="D28" s="70" t="s">
+        <v>350</v>
+      </c>
+      <c r="E28" s="70" t="s">
+        <v>351</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>337</v>
+      </c>
+      <c r="G28" s="85" t="s">
+        <v>316</v>
       </c>
       <c r="H28" s="11"/>
       <c r="I28" s="61"/>
     </row>
-    <row r="29" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="10"/>
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
-      <c r="D29" s="57" t="s">
-        <v>314</v>
+      <c r="D29" s="70" t="s">
+        <v>350</v>
       </c>
       <c r="E29" s="70" t="s">
-        <v>324</v>
-      </c>
-      <c r="F29" s="14"/>
-      <c r="G29" s="68" t="s">
-        <v>126</v>
+        <v>351</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>337</v>
+      </c>
+      <c r="G29" s="61" t="s">
+        <v>16</v>
       </c>
       <c r="H29" s="11"/>
       <c r="I29" s="61"/>
     </row>
-    <row r="30" spans="1:9" s="53" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A30" s="50"/>
-      <c r="B30" s="50"/>
-      <c r="C30" s="50" t="s">
-        <v>9</v>
-      </c>
-      <c r="D30" s="51" t="s">
-        <v>199</v>
-      </c>
-      <c r="E30" s="52" t="s">
-        <v>301</v>
-      </c>
-      <c r="F30" s="52"/>
-      <c r="G30" s="50"/>
-      <c r="H30" s="50"/>
-      <c r="I30" s="50" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="10"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="57" t="s">
+        <v>305</v>
+      </c>
+      <c r="E30" s="57" t="s">
+        <v>322</v>
+      </c>
+      <c r="F30" s="14"/>
+      <c r="G30" s="61" t="s">
+        <v>318</v>
+      </c>
+      <c r="H30" s="11"/>
+      <c r="I30" s="61"/>
+    </row>
+    <row r="31" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10"/>
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="14"/>
+      <c r="D31" s="57" t="s">
+        <v>314</v>
+      </c>
+      <c r="E31" s="70" t="s">
+        <v>323</v>
+      </c>
       <c r="F31" s="14"/>
-      <c r="G31" s="61" t="s">
-        <v>63</v>
+      <c r="G31" s="68" t="s">
+        <v>126</v>
       </c>
       <c r="H31" s="11"/>
-      <c r="I31" s="68"/>
-    </row>
-    <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="10"/>
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="61" t="s">
-        <v>302</v>
-      </c>
-      <c r="H32" s="11"/>
-      <c r="I32" s="61"/>
-    </row>
-    <row r="33" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="I31" s="61"/>
+    </row>
+    <row r="32" spans="1:9" s="53" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A32" s="50"/>
+      <c r="B32" s="50"/>
+      <c r="C32" s="50" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="51" t="s">
+        <v>199</v>
+      </c>
+      <c r="E32" s="52" t="s">
+        <v>301</v>
+      </c>
+      <c r="F32" s="52"/>
+      <c r="G32" s="50"/>
+      <c r="H32" s="50"/>
+      <c r="I32" s="50" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="10"/>
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
       <c r="D33" s="12"/>
       <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
+      <c r="F33" s="88" t="s">
+        <v>352</v>
+      </c>
       <c r="G33" s="61" t="s">
-        <v>303</v>
+        <v>63</v>
       </c>
       <c r="H33" s="11"/>
-      <c r="I33" s="61"/>
-    </row>
-    <row r="34" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A34" s="50"/>
-      <c r="B34" s="50"/>
-      <c r="C34" s="50" t="s">
-        <v>9</v>
-      </c>
-      <c r="D34" s="51" t="s">
-        <v>199</v>
-      </c>
-      <c r="E34" s="52" t="s">
-        <v>271</v>
-      </c>
-      <c r="F34" s="52"/>
-      <c r="G34" s="50"/>
-      <c r="H34" s="50"/>
-      <c r="I34" s="50" t="s">
-        <v>13</v>
-      </c>
+      <c r="I33" s="68"/>
+    </row>
+    <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="10"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="88" t="s">
+        <v>353</v>
+      </c>
+      <c r="G34" s="61" t="s">
+        <v>302</v>
+      </c>
+      <c r="H34" s="11"/>
+      <c r="I34" s="61"/>
     </row>
     <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="10"/>
       <c r="B35" s="11"/>
       <c r="C35" s="11"/>
-      <c r="D35" s="57"/>
-      <c r="E35" s="57" t="s">
-        <v>325</v>
-      </c>
+      <c r="D35" s="12"/>
+      <c r="E35" s="14"/>
       <c r="F35" s="14"/>
       <c r="G35" s="61" t="s">
-        <v>315</v>
+        <v>303</v>
       </c>
       <c r="H35" s="11"/>
       <c r="I35" s="61"/>
     </row>
-    <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="10"/>
-      <c r="B36" s="11"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="61"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="61"/>
+    <row r="36" spans="1:9" s="53" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A36" s="50"/>
+      <c r="B36" s="50"/>
+      <c r="C36" s="50" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" s="51" t="s">
+        <v>199</v>
+      </c>
+      <c r="E36" s="52" t="s">
+        <v>271</v>
+      </c>
+      <c r="F36" s="52"/>
+      <c r="G36" s="50"/>
+      <c r="H36" s="50"/>
+      <c r="I36" s="50" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="37" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="10"/>
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="14"/>
+      <c r="D37" s="57"/>
+      <c r="E37" s="57" t="s">
+        <v>324</v>
+      </c>
       <c r="F37" s="14"/>
-      <c r="G37" s="61"/>
+      <c r="G37" s="61" t="s">
+        <v>315</v>
+      </c>
       <c r="H37" s="11"/>
       <c r="I37" s="61"/>
     </row>
@@ -13093,8 +13186,30 @@
       <c r="I999" s="61"/>
     </row>
     <row r="1000" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1000" s="10"/>
+      <c r="B1000" s="11"/>
+      <c r="C1000" s="11"/>
       <c r="D1000" s="12"/>
       <c r="E1000" s="14"/>
+      <c r="F1000" s="14"/>
+      <c r="G1000" s="61"/>
+      <c r="H1000" s="11"/>
+      <c r="I1000" s="61"/>
+    </row>
+    <row r="1001" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1001" s="10"/>
+      <c r="B1001" s="11"/>
+      <c r="C1001" s="11"/>
+      <c r="D1001" s="12"/>
+      <c r="E1001" s="14"/>
+      <c r="F1001" s="14"/>
+      <c r="G1001" s="61"/>
+      <c r="H1001" s="11"/>
+      <c r="I1001" s="61"/>
+    </row>
+    <row r="1002" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="D1002" s="12"/>
+      <c r="E1002" s="14"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I1"/>
@@ -13102,7 +13217,7 @@
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.3" footer="0.3"/>
   <pageSetup fitToWidth="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="17" max="16383" man="1"/>
+    <brk id="19" max="16383" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
@@ -37659,17 +37774,17 @@
       <c r="I32" s="12"/>
     </row>
     <row r="33" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A33" s="99" t="s">
+      <c r="A33" s="103" t="s">
         <v>103</v>
       </c>
-      <c r="B33" s="100"/>
-      <c r="C33" s="100"/>
-      <c r="D33" s="100"/>
-      <c r="E33" s="100"/>
-      <c r="F33" s="100"/>
-      <c r="G33" s="100"/>
-      <c r="H33" s="100"/>
-      <c r="I33" s="100"/>
+      <c r="B33" s="104"/>
+      <c r="C33" s="104"/>
+      <c r="D33" s="104"/>
+      <c r="E33" s="104"/>
+      <c r="F33" s="104"/>
+      <c r="G33" s="104"/>
+      <c r="H33" s="104"/>
+      <c r="I33" s="104"/>
     </row>
     <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="10"/>
@@ -49004,17 +49119,17 @@
       <c r="I18" s="12"/>
     </row>
     <row r="19" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A19" s="99" t="s">
+      <c r="A19" s="103" t="s">
         <v>103</v>
       </c>
-      <c r="B19" s="100"/>
-      <c r="C19" s="100"/>
-      <c r="D19" s="100"/>
-      <c r="E19" s="100"/>
-      <c r="F19" s="100"/>
-      <c r="G19" s="100"/>
-      <c r="H19" s="100"/>
-      <c r="I19" s="100"/>
+      <c r="B19" s="104"/>
+      <c r="C19" s="104"/>
+      <c r="D19" s="104"/>
+      <c r="E19" s="104"/>
+      <c r="F19" s="104"/>
+      <c r="G19" s="104"/>
+      <c r="H19" s="104"/>
+      <c r="I19" s="104"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>

</xml_diff>